<commit_message>
Prep for new 3D modeling branch.
</commit_message>
<xml_diff>
--- a/admin_color_tools/Colors_Master.xlsx
+++ b/admin_color_tools/Colors_Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usRyaTim\Onedrive - LEGO\Documents\brickr\Colors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usRyaTim\Onedrive - LEGO\Documents\brickr\admin_color_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{7ECD4211-67B7-488D-B3AD-E057FA58E385}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D18FC5E9-F768-4236-ADA1-E219070EED5A}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{7ECD4211-67B7-488D-B3AD-E057FA58E385}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9B004BAE-AC8E-4167-8D82-7C1F0E31B0C1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A30B29F7-B580-406F-8677-17DD8856CE58}"/>
   </bookViews>
@@ -979,9 +979,9 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add transparent colors to lego_colors. Filter these out for mosaic matching.
</commit_message>
<xml_diff>
--- a/admin_color_tools/Colors_Master.xlsx
+++ b/admin_color_tools/Colors_Master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usRyaTim\Onedrive - LEGO\Documents\brickr\admin_color_tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{7ECD4211-67B7-488D-B3AD-E057FA58E385}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{9B004BAE-AC8E-4167-8D82-7C1F0E31B0C1}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{7ECD4211-67B7-488D-B3AD-E057FA58E385}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5B82EC2C-398D-4A6E-8449-CEB10C58DB8C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A30B29F7-B580-406F-8677-17DD8856CE58}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{A30B29F7-B580-406F-8677-17DD8856CE58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>LEGONo</t>
   </si>
@@ -135,30 +135,6 @@
     <t>Transparent</t>
   </si>
   <si>
-    <t>Tr. Red</t>
-  </si>
-  <si>
-    <t>Tr. Lg blue</t>
-  </si>
-  <si>
-    <t>Tr. Blue</t>
-  </si>
-  <si>
-    <t>Tr. Yellow</t>
-  </si>
-  <si>
-    <t>Tr. Flu. Reddish orange</t>
-  </si>
-  <si>
-    <t>Tr. Green</t>
-  </si>
-  <si>
-    <t>Tr. Flu. Green</t>
-  </si>
-  <si>
-    <t>Tr. Brown</t>
-  </si>
-  <si>
     <t>Aqua</t>
   </si>
   <si>
@@ -189,9 +165,6 @@
     <t>Silver Metallic</t>
   </si>
   <si>
-    <t>Tr. Bright Green</t>
-  </si>
-  <si>
     <t>Universal</t>
   </si>
   <si>
@@ -201,12 +174,6 @@
     <t>Special</t>
   </si>
   <si>
-    <t>Tr. Medium violet</t>
-  </si>
-  <si>
-    <t>Tr. Bright violet</t>
-  </si>
-  <si>
     <t>Light royal blue</t>
   </si>
   <si>
@@ -238,6 +205,42 @@
   </si>
   <si>
     <t>Light nougat</t>
+  </si>
+  <si>
+    <t>Tr. light blue</t>
+  </si>
+  <si>
+    <t>Tr. red</t>
+  </si>
+  <si>
+    <t>Tr. blue</t>
+  </si>
+  <si>
+    <t>Tr. yellow</t>
+  </si>
+  <si>
+    <t>Tr. green</t>
+  </si>
+  <si>
+    <t>Tr. fl red orange</t>
+  </si>
+  <si>
+    <t>Tr. fl green</t>
+  </si>
+  <si>
+    <t>Tr. brown</t>
+  </si>
+  <si>
+    <t>Tr. bright orange</t>
+  </si>
+  <si>
+    <t>Tr. medium violet</t>
+  </si>
+  <si>
+    <t>Tr. bright violet</t>
+  </si>
+  <si>
+    <t>Tr. bright green</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="44">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -510,6 +513,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8D0A"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD246"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -526,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -656,6 +671,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,6 +683,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFAFD246"/>
+      <color rgb="FFFF8D0A"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FF33CCCC"/>
     </mruColors>
@@ -976,12 +997,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF3980FF-9756-4A4E-962F-50E7DE1C9AD8}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
+      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -989,7 +1010,8 @@
     <col min="1" max="1" width="9.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="4.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
     <col min="8" max="9" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1017,19 +1039,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1050,7 +1072,7 @@
         <v>244</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1" t="b">
         <v>1</v>
@@ -1083,7 +1105,7 @@
         <v>141</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1" t="b">
         <v>1</v>
@@ -1116,7 +1138,7 @@
         <v>90</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H4" s="1" t="b">
         <v>1</v>
@@ -1149,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1" t="b">
         <v>1</v>
@@ -1182,7 +1204,7 @@
         <v>168</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H6" s="1" t="b">
         <v>1</v>
@@ -1215,7 +1237,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H7" s="1" t="b">
         <v>1</v>
@@ -1248,7 +1270,7 @@
         <v>52</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H8" s="1" t="b">
         <v>1</v>
@@ -1281,7 +1303,7 @@
         <v>43</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H9" s="1" t="b">
         <v>1</v>
@@ -1314,7 +1336,7 @@
         <v>65</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H10" s="1" t="b">
         <v>1</v>
@@ -1347,7 +1369,7 @@
         <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H11" s="1" t="b">
         <v>1</v>
@@ -1380,7 +1402,7 @@
         <v>238</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H12" s="1" t="b">
         <v>1</v>
@@ -1400,7 +1422,7 @@
         <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="2">
@@ -1413,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H13" s="1" t="b">
         <v>1</v>
@@ -1433,7 +1455,7 @@
         <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C14" s="33"/>
       <c r="D14" s="2">
@@ -1446,7 +1468,7 @@
         <v>237</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H14" s="1" t="b">
         <v>1</v>
@@ -1466,7 +1488,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="2">
@@ -1479,7 +1501,7 @@
         <v>184</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H15" s="1" t="b">
         <v>1</v>
@@ -1499,7 +1521,7 @@
         <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="C16" s="35"/>
       <c r="D16" s="2">
@@ -1512,7 +1534,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H16" s="1" t="b">
         <v>1</v>
@@ -1532,7 +1554,7 @@
         <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="2">
@@ -1545,7 +1567,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H17" s="1" t="b">
         <v>1</v>
@@ -1565,7 +1587,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="2">
@@ -1578,7 +1600,7 @@
         <v>100</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H18" s="1" t="b">
         <v>1</v>
@@ -1598,7 +1620,7 @@
         <v>49</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C19" s="38"/>
       <c r="D19" s="2">
@@ -1611,7 +1633,7 @@
         <v>91</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H19" s="1" t="b">
         <v>1</v>
@@ -1644,7 +1666,7 @@
         <v>200</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H20" s="1" t="b">
         <v>1</v>
@@ -1677,7 +1699,7 @@
         <v>35</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H21" s="1" t="b">
         <v>1</v>
@@ -1710,7 +1732,7 @@
         <v>148</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H22" s="1" t="b">
         <v>1</v>
@@ -1730,7 +1752,7 @@
         <v>111</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="2">
@@ -1743,7 +1765,7 @@
         <v>158</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H23" s="1" t="b">
         <v>1</v>
@@ -1763,7 +1785,7 @@
         <v>113</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="2">
@@ -1776,7 +1798,7 @@
         <v>207</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H24" s="1" t="b">
         <v>1</v>
@@ -1809,7 +1831,7 @@
         <v>24</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H25" s="1" t="b">
         <v>1</v>
@@ -1842,7 +1864,7 @@
         <v>118</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H26" s="1" t="b">
         <v>1</v>
@@ -1862,7 +1884,7 @@
         <v>126</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="2">
@@ -1875,7 +1897,7 @@
         <v>184</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H27" s="1" t="b">
         <v>1</v>
@@ -1908,7 +1930,7 @@
         <v>154</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H28" s="1" t="b">
         <v>1</v>
@@ -1941,7 +1963,7 @@
         <v>98</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H29" s="1" t="b">
         <v>1</v>
@@ -1974,7 +1996,7 @@
         <v>90</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H30" s="1" t="b">
         <v>1</v>
@@ -2007,7 +2029,7 @@
         <v>26</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H31" s="1" t="b">
         <v>1</v>
@@ -2040,7 +2062,7 @@
         <v>124</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H32" s="1" t="b">
         <v>1</v>
@@ -2073,7 +2095,7 @@
         <v>18</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H33" s="1" t="b">
         <v>1</v>
@@ -2090,29 +2112,29 @@
     </row>
     <row r="34" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="23"/>
+        <v>68</v>
+      </c>
+      <c r="C34" s="45"/>
       <c r="D34" s="2">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="E34" s="2">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="F34" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H34" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="1" t="b">
         <v>0</v>
@@ -2123,23 +2145,23 @@
     </row>
     <row r="35" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="C35" s="23"/>
       <c r="D35" s="2">
-        <v>95</v>
+        <v>252</v>
       </c>
       <c r="E35" s="2">
-        <v>49</v>
+        <v>172</v>
       </c>
       <c r="F35" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H35" s="1" t="b">
         <v>1</v>
@@ -2156,23 +2178,23 @@
     </row>
     <row r="36" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="25"/>
+        <v>28</v>
+      </c>
+      <c r="C36" s="24"/>
       <c r="D36" s="2">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="E36" s="2">
-        <v>150</v>
+        <v>49</v>
       </c>
       <c r="F36" s="2">
-        <v>150</v>
+        <v>9</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H36" s="1" t="b">
         <v>1</v>
@@ -2189,23 +2211,23 @@
     </row>
     <row r="37" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="26"/>
+        <v>29</v>
+      </c>
+      <c r="C37" s="25"/>
       <c r="D37" s="2">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="E37" s="2">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="F37" s="2">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="H37" s="1" t="b">
         <v>1</v>
@@ -2222,23 +2244,23 @@
     </row>
     <row r="38" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C38" s="26"/>
       <c r="D38" s="2">
-        <v>157</v>
+        <v>100</v>
       </c>
       <c r="E38" s="2">
-        <v>195</v>
+        <v>100</v>
       </c>
       <c r="F38" s="2">
-        <v>247</v>
+        <v>100</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H38" s="1" t="b">
         <v>1</v>
@@ -2255,23 +2277,23 @@
     </row>
     <row r="39" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="27"/>
+        <v>49</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="2">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="E39" s="2">
-        <v>80</v>
+        <v>195</v>
       </c>
       <c r="F39" s="2">
-        <v>155</v>
+        <v>247</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H39" s="1" t="b">
         <v>1</v>
@@ -2288,23 +2310,23 @@
     </row>
     <row r="40" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="C40" s="27"/>
       <c r="D40" s="2">
-        <v>255</v>
+        <v>200</v>
       </c>
       <c r="E40" s="2">
-        <v>158</v>
+        <v>80</v>
       </c>
       <c r="F40" s="2">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="H40" s="1" t="b">
         <v>1</v>
@@ -2321,23 +2343,23 @@
     </row>
     <row r="41" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="29"/>
+        <v>32</v>
+      </c>
+      <c r="C41" s="28"/>
       <c r="D41" s="2">
         <v>255</v>
       </c>
       <c r="E41" s="2">
-        <v>236</v>
+        <v>158</v>
       </c>
       <c r="F41" s="2">
-        <v>108</v>
+        <v>205</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H41" s="1" t="b">
         <v>1</v>
@@ -2354,23 +2376,23 @@
     </row>
     <row r="42" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>268</v>
+        <v>226</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="C42" s="29"/>
       <c r="D42" s="2">
-        <v>68</v>
+        <v>255</v>
       </c>
       <c r="E42" s="2">
-        <v>26</v>
+        <v>236</v>
       </c>
       <c r="F42" s="2">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H42" s="1" t="b">
         <v>1</v>
@@ -2387,23 +2409,23 @@
     </row>
     <row r="43" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C43" s="30"/>
       <c r="D43" s="2">
-        <v>225</v>
+        <v>68</v>
       </c>
       <c r="E43" s="2">
-        <v>190</v>
+        <v>26</v>
       </c>
       <c r="F43" s="2">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H43" s="1" t="b">
         <v>1</v>
@@ -2420,23 +2442,23 @@
     </row>
     <row r="44" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="E44" s="2">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="F44" s="2">
-        <v>34</v>
+        <v>161</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H44" s="1" t="b">
         <v>1</v>
@@ -2448,99 +2470,100 @@
         <v>0</v>
       </c>
       <c r="K44" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
+        <v>175</v>
+      </c>
+      <c r="E45" s="2">
+        <v>133</v>
+      </c>
+      <c r="F45" s="2">
+        <v>34</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H45" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>308</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2">
         <v>53</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E46" s="2">
         <v>33</v>
       </c>
-      <c r="F45" s="2">
-        <v>0</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>311</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="1">
+      <c r="B47" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="46"/>
+      <c r="D47" s="1">
         <v>175</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E47" s="1">
         <v>210</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F47" s="1">
         <v>70</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H46" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I46" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="J46" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K46" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>312</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2">
-        <v>170</v>
-      </c>
-      <c r="E47" s="2">
-        <v>125</v>
-      </c>
-      <c r="F47" s="2">
-        <v>85</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>57</v>
+      <c r="G47" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="H47" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I47" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" s="1" t="b">
         <v>0</v>
@@ -2551,23 +2574,23 @@
     </row>
     <row r="48" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="E48" s="2">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="F48" s="2">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H48" s="1" t="b">
         <v>1</v>
@@ -2579,28 +2602,28 @@
         <v>0</v>
       </c>
       <c r="K48" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="E49" s="2">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="F49" s="2">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H49" s="1" t="b">
         <v>1</v>
@@ -2617,23 +2640,23 @@
     </row>
     <row r="50" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2">
+        <v>73</v>
+      </c>
+      <c r="E50" s="2">
         <v>70</v>
       </c>
-      <c r="E50" s="2">
-        <v>155</v>
-      </c>
       <c r="F50" s="2">
-        <v>195</v>
+        <v>68</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H50" s="1" t="b">
         <v>1</v>
@@ -2645,28 +2668,28 @@
         <v>0</v>
       </c>
       <c r="K50" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="E51" s="2">
+        <v>155</v>
+      </c>
+      <c r="F51" s="2">
         <v>195</v>
       </c>
-      <c r="F51" s="2">
-        <v>226</v>
-      </c>
       <c r="G51" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H51" s="1" t="b">
         <v>1</v>
@@ -2683,23 +2706,23 @@
     </row>
     <row r="52" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2">
-        <v>211</v>
+        <v>104</v>
       </c>
       <c r="E52" s="2">
-        <v>242</v>
+        <v>195</v>
       </c>
       <c r="F52" s="2">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H52" s="1" t="b">
         <v>1</v>
@@ -2716,23 +2739,23 @@
     </row>
     <row r="53" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="E53" s="2">
-        <v>118</v>
+        <v>242</v>
       </c>
       <c r="F53" s="2">
-        <v>174</v>
+        <v>234</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H53" s="1" t="b">
         <v>1</v>
@@ -2749,23 +2772,23 @@
     </row>
     <row r="54" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
-        <v>205</v>
+        <v>154</v>
       </c>
       <c r="E54" s="2">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="F54" s="2">
-        <v>222</v>
+        <v>174</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H54" s="1" t="b">
         <v>1</v>
@@ -2782,23 +2805,23 @@
     </row>
     <row r="55" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="E55" s="2">
-        <v>249</v>
+        <v>164</v>
       </c>
       <c r="F55" s="2">
-        <v>154</v>
+        <v>222</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H55" s="1" t="b">
         <v>1</v>
@@ -2815,23 +2838,23 @@
     </row>
     <row r="56" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2">
-        <v>245</v>
+        <v>226</v>
       </c>
       <c r="E56" s="2">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F56" s="2">
-        <v>214</v>
+        <v>154</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="H56" s="1" t="b">
         <v>1</v>
@@ -2840,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="J56" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56" s="1" t="b">
         <v>0</v>
@@ -2848,74 +2871,107 @@
     </row>
     <row r="57" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2">
+        <v>245</v>
+      </c>
+      <c r="E57" s="2">
+        <v>243</v>
+      </c>
+      <c r="F57" s="2">
+        <v>214</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H57" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K57" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>330</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2">
         <v>139</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E58" s="2">
         <v>132</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F58" s="2">
         <v>79</v>
       </c>
-      <c r="G57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H57" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I57" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J57" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K57" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="G58" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>353</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="44"/>
-      <c r="D58" s="1">
+      <c r="B59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="44"/>
+      <c r="D59" s="1">
         <v>240</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E59" s="1">
         <v>109</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F59" s="1">
         <v>120</v>
       </c>
-      <c r="G58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H58" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I58" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J58" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K58" s="1" t="b">
+      <c r="G59" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H59" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K57">
-    <sortCondition descending="1" ref="H2:H57"/>
-    <sortCondition ref="A2:A57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K58">
+    <sortCondition descending="1" ref="H2:H58"/>
+    <sortCondition ref="A2:A58"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>